<commit_message>
updated on 31st 2024
</commit_message>
<xml_diff>
--- a/static/files/products_export.xlsx
+++ b/static/files/products_export.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>brand_name</t>
   </si>
@@ -43,22 +43,34 @@
     <t>image_path</t>
   </si>
   <si>
-    <t>Royal Stag</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>8901088200073</t>
-  </si>
-  <si>
-    <t>Whisky</t>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>0277</t>
+  </si>
+  <si>
+    <t>8901544027077</t>
+  </si>
+  <si>
+    <t>8901544027060</t>
+  </si>
+  <si>
+    <t>8901544027039</t>
+  </si>
+  <si>
+    <t>WHISKY</t>
   </si>
   <si>
     <t>180</t>
   </si>
   <si>
-    <t>static/uploads/3D_design_logo_for_New_Pavan_Restaurant___Bar_with_a_beverages_theme_on_a_white_background-removebg-preview_1.png</t>
+    <t>375</t>
+  </si>
+  <si>
+    <t>750</t>
+  </si>
+  <si>
+    <t>static/uploads/Default.png</t>
   </si>
 </sst>
 </file>
@@ -416,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,22 +474,80 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>320</v>
       </c>
       <c r="E2">
-        <v>150</v>
+        <v>320</v>
       </c>
       <c r="F2">
-        <v>200</v>
+        <v>370</v>
       </c>
       <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="D3">
+        <v>730</v>
+      </c>
+      <c r="E3">
+        <v>730</v>
+      </c>
+      <c r="F3">
+        <v>740</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="D4">
+        <v>1450</v>
+      </c>
+      <c r="E4">
+        <v>1450</v>
+      </c>
+      <c r="F4">
+        <v>1480</v>
+      </c>
+      <c r="G4" t="s">
         <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>